<commit_message>
SML FHIR IG with the latest SML CDA IG download
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/practitioner-dh-base-1.xlsx
+++ b/output/SharedMedicinesList/practitioner-dh-base-1.xlsx
@@ -9696,7 +9696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" hidden="true">
+    <row r="75">
       <c r="A75" t="s" s="2">
         <v>318</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>42</v>
       </c>
       <c r="G75" t="s" s="2">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H75" t="s" s="2">
         <v>40</v>
@@ -9807,7 +9807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" hidden="true">
+    <row r="76">
       <c r="A76" t="s" s="2">
         <v>323</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>52</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>40</v>
@@ -9916,7 +9916,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" hidden="true">
+    <row r="77">
       <c r="A77" t="s" s="2">
         <v>330</v>
       </c>
@@ -9932,7 +9932,7 @@
         <v>52</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>40</v>
@@ -10027,7 +10027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" hidden="true">
+    <row r="78">
       <c r="A78" t="s" s="2">
         <v>336</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>52</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>40</v>

</xml_diff>